<commit_message>
updated identity_schema_id & apptyp_code
Signed-off-by: GOKULRAJ136 <110164849+GOKULRAJ136@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/identity_schema.xlsx
+++ b/mosip_master/xlsx/identity_schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yash.mohan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gokulraj\Documents\GitHub\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF15F67C-E609-4D9C-ABB1-13CF793BAFD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE57EE3D-7D7B-4E50-A44C-ED46C4441A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1063,7 +1063,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1082,9 +1082,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1458,8 +1455,8 @@
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="7">
-        <v>1001</v>
+      <c r="B2" s="1">
+        <v>1002</v>
       </c>
       <c r="C2" s="1">
         <v>0.1</v>
@@ -1490,8 +1487,8 @@
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="7">
-        <v>1002</v>
+      <c r="B3" s="1">
+        <v>1001</v>
       </c>
       <c r="C3" s="1">
         <v>0.2</v>

</xml_diff>

<commit_message>
removed array of handle identity schema
Signed-off-by: dhanendra06 <dhanendra.tech@gmail.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/identity_schema.xlsx
+++ b/mosip_master/xlsx/identity_schema.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gokulraj\Documents\GitHub\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lapBkp\projects\mosip\test8\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE57EE3D-7D7B-4E50-A44C-ED46C4441A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69592AFE-6B4F-43C0-B369-32D9000979DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>lang_code</t>
   </si>
@@ -524,490 +524,12 @@
 	}
 }</t>
   </si>
-  <si>
-    <t>Mosip Sample identity for handle</t>
-  </si>
-  <si>
-    <t>Mosip Identity for handle</t>
-  </si>
-  <si>
-    <t>{
-    "$schema": "http:\/\/json-schema.org\/draft-07\/schema#",
-    "description": "MOSIP Sample identity",
-    "additionalProperties": false,
-    "title": "MOSIP identity",
-    "type": "object",
-    "definitions": {
-        "simpleType": {
-            "uniqueItems": true,
-            "additionalItems": false,
-            "type": "array",
-            "items": {
-                "additionalProperties": false,
-                "type": "object",
-                "required": [
-                    "language",
-                    "value"
-                ],
-                "properties": {
-                    "language": {
-                        "type": "string"
-                    },
-                    "value": {
-                        "type": "string"
-                    }
-                }
-            }
-        },
-        "taggedListType": {
-            "uniqueItems": true,
-            "additionalItems": false,
-            "type": "array",
-            "items": {
-                "additionalProperties": false,
-                "type": "object",
-                "required": [
-                    "value"
-                ],
-                "properties": {
-                    "value": {
-                        "type": "string"
-                    },
-                    "tags": {
-                        "uniqueItems": true,
-                        "type": "array",
-                        "items": {
-                            "type": "string",
-                            "enum": [
-                                "notification",
-                                "handle"
-                            ]
-                        }
-                    }
-                }
-            }
-        },
-        "hashType": {
-            "additionalProperties": false,
-            "type": "object",
-            "properties": {
-                "hash": {
-                    "type": "string"
-                },
-                "salt": {
-                    "type": "string"
-                }
-            }
-        },
-        "documentType": {
-            "additionalProperties": false,
-            "type": "object",
-            "properties": {
-                "format": {
-                    "type": "string"
-                },
-                "type": {
-                    "type": "string"
-                },
-                "value": {
-                    "type": "string"
-                },
-                "refNumber": {
-                    "type": [
-                        "string",
-                        "null"
-                    ]
-                }
-            }
-        },
-        "biometricsType": {
-            "additionalProperties": false,
-            "type": "object",
-            "properties": {
-                "format": {
-                    "type": "string"
-                },
-                "version": {
-                    "type": "number",
-                    "minimum": 0
-                },
-                "value": {
-                    "type": "string"
-                }
-            }
-        }
-    },
-    "properties": {
-        "identity": {
-            "additionalProperties": false,
-            "type": "object",
-            "required": [
-                "IDSchemaVersion",
-                "fullName",
-                "dateOfBirth",
-                "gender",
-                "addressLine1",
-                "addressLine2",
-                "addressLine3",
-                "region",
-                "province",
-                "city",
-                "zone",
-                "postalCode",
-                "phone",
-                "email",
-                "proofOfIdentity",
-                "individualBiometrics"
-            ],
-            "properties": {
-                "proofOfAddress": {
-                    "bioAttributes": [],
-                    "fieldCategory": "pvt",
-                    "format": "none",
-                    "fieldType": "default",
-                    "$ref": "#\/definitions\/documentType"
-                },
-                "gender": {
-                    "bioAttributes": [],
-                    "fieldCategory": "pvt",
-                    "format": "",
-                    "fieldType": "default",
-                    "$ref": "#\/definitions\/simpleType"
-                },
-                "city": {
-                    "bioAttributes": [],
-                    "validators": [
-                        {
-                            "validator": "^(?=.{0,50}$).*",
-                            "arguments": [],
-                            "type": "regex"
-                        }
-                    ],
-                    "fieldCategory": "pvt",
-                    "format": "none",
-                    "fieldType": "default",
-                    "$ref": "#\/definitions\/simpleType"
-                },
-                "postalCode": {
-                    "bioAttributes": [],
-                    "validators": [
-                        {
-                            "validator": "^[(?i)A-Z0-9]{5}$|^NA$",
-                            "arguments": [],
-                            "type": "regex"
-                        }
-                    ],
-                    "fieldCategory": "pvt",
-                    "format": "none",
-                    "type": "string",
-                    "fieldType": "default"
-                },
-                "proofOfException-1": {
-                    "bioAttributes": [],
-                    "fieldCategory": "evidence",
-                    "format": "none",
-                    "fieldType": "default",
-                    "$ref": "#\/definitions\/documentType"
-                },
-                "referenceIdentityNumber": {
-                    "bioAttributes": [],
-                    "validators": [
-                        {
-                            "validator": "^([0-9]{10,30})$",
-                            "arguments": [],
-                            "type": "regex"
-                        }
-                    ],
-                    "fieldCategory": "pvt",
-                    "format": "kyc",
-                    "type": "string",
-                    "fieldType": "default"
-                },
-                "individualBiometrics": {
-                    "bioAttributes": [
-                        "leftEye",
-                        "rightEye",
-                        "rightIndex",
-                        "rightLittle",
-                        "rightRing",
-                        "rightMiddle",
-                        "leftIndex",
-                        "leftLittle",
-                        "leftRing",
-                        "leftMiddle",
-                        "leftThumb",
-                        "rightThumb",
-                        "face"
-                    ],
-                    "fieldCategory": "pvt",
-                    "format": "none",
-                    "fieldType": "default",
-                    "$ref": "#\/definitions\/biometricsType"
-                },
-                "province": {
-                    "bioAttributes": [],
-                    "validators": [
-                        {
-                            "validator": "^(?=.{0,50}$).*",
-                            "arguments": [],
-                            "type": "regex"
-                        }
-                    ],
-                    "fieldCategory": "pvt",
-                    "format": "none",
-                    "fieldType": "default",
-                    "$ref": "#\/definitions\/simpleType"
-                },
-                "zone": {
-                    "bioAttributes": [],
-                    "fieldCategory": "pvt",
-                    "format": "none",
-                    "fieldType": "default",
-                    "$ref": "#\/definitions\/simpleType"
-                },
-                "proofOfDateOfBirth": {
-                    "bioAttributes": [],
-                    "fieldCategory": "pvt",
-                    "format": "none",
-                    "fieldType": "default",
-                    "$ref": "#\/definitions\/documentType"
-                },
-                "addressLine1": {
-                    "bioAttributes": [],
-                    "validators": [
-                        {
-                            "validator": "^(?=.{0,50}$).*",
-                            "arguments": [],
-                            "type": "regex"
-                        }
-                    ],
-                    "fieldCategory": "pvt",
-                    "format": "none",
-                    "fieldType": "default",
-                    "$ref": "#\/definitions\/simpleType"
-                },
-                "addressLine2": {
-                    "bioAttributes": [],
-                    "validators": [
-                        {
-                            "validator": "^(?=.{3,50}$).*",
-                            "arguments": [],
-                            "type": "regex"
-                        }
-                    ],
-                    "fieldCategory": "pvt",
-                    "format": "none",
-                    "fieldType": "default",
-                    "$ref": "#\/definitions\/simpleType"
-                },
-                "residenceStatus": {
-                    "bioAttributes": [],
-                    "fieldCategory": "kyc",
-                    "format": "none",
-                    "fieldType": "default",
-                    "$ref": "#\/definitions\/simpleType"
-                },
-                "addressLine3": {
-                    "bioAttributes": [],
-                    "validators": [
-                        {
-                            "validator": "^(?=.{3,50}$).*",
-                            "arguments": [],
-                            "type": "regex"
-                        }
-                    ],
-                    "fieldCategory": "pvt",
-                    "format": "none",
-                    "fieldType": "default",
-                    "$ref": "#\/definitions\/simpleType"
-                },
-                "email": {
-                    "bioAttributes": [],
-                    "validators": [
-                        {
-                            "validator": "^[A-Za-z0-9_\\-]+(\\.[A-Za-z0-9_]+)*@[A-Za-z0-9_-]+(\\.[A-Za-z0-9_]+)*(\\.[a-zA-Z]{2,})$",
-                            "arguments": [],
-                            "type": "regex"
-                        }
-                    ],
-                    "fieldCategory": "pvt",
-                    "format": "none",
-                    "type": "string",
-                    "fieldType": "default"
-                },
-                "introducerRID": {
-                    "bioAttributes": [],
-                    "fieldCategory": "evidence",
-                    "format": "none",
-                    "type": "string",
-                    "fieldType": "default"
-                },
-                "introducerBiometrics": {
-                    "bioAttributes": [
-                        "leftEye",
-                        "rightEye",
-                        "rightIndex",
-                        "rightLittle",
-                        "rightRing",
-                        "rightMiddle",
-                        "leftIndex",
-                        "leftLittle",
-                        "leftRing",
-                        "leftMiddle",
-                        "leftThumb",
-                        "rightThumb",
-                        "face"
-                    ],
-                    "fieldCategory": "pvt",
-                    "format": "none",
-                    "fieldType": "default",
-                    "$ref": "#\/definitions\/biometricsType"
-                },
-                "fullName": {
-                    "bioAttributes": [],
-                    "validators": [
-                        {
-                            "validator": "^(?=.{3,50}$).*",
-                            "arguments": [],
-                            "type": "regex"
-                        }
-                    ],
-                    "fieldCategory": "pvt",
-                    "format": "none",
-                    "fieldType": "default",
-                    "$ref": "#\/definitions\/simpleType"
-                },
-                "dateOfBirth": {
-                    "bioAttributes": [],
-                    "validators": [
-                        {
-                            "validator": "^(1869|18[7-9][0-9]|19[0-9][0-9]|20[0-9][0-9])\/([0][1-9]|1[0-2])\/([0][1-9]|[1-2][0-9]|3[01])$",
-                            "arguments": [],
-                            "type": "regex"
-                        }
-                    ],
-                    "fieldCategory": "pvt",
-                    "format": "none",
-                    "type": "string",
-                    "fieldType": "default"
-                },
-                "individualAuthBiometrics": {
-                    "bioAttributes": [
-                        "leftEye",
-                        "rightEye",
-                        "rightIndex",
-                        "rightLittle",
-                        "rightRing",
-                        "rightMiddle",
-                        "leftIndex",
-                        "leftLittle",
-                        "leftRing",
-                        "leftMiddle",
-                        "leftThumb",
-                        "rightThumb",
-                        "face"
-                    ],
-                    "fieldCategory": "pvt",
-                    "format": "none",
-                    "fieldType": "default",
-                    "$ref": "#\/definitions\/biometricsType"
-                },
-                "introducerUIN": {
-                    "bioAttributes": [],
-                    "fieldCategory": "evidence",
-                    "format": "none",
-                    "type": "string",
-                    "fieldType": "default"
-                },
-                "proofOfIdentity": {
-                    "bioAttributes": [],
-                    "fieldCategory": "pvt",
-                    "format": "none",
-                    "fieldType": "default",
-                    "$ref": "#\/definitions\/documentType"
-                },
-                "IDSchemaVersion": {
-                    "bioAttributes": [],
-                    "fieldCategory": "none",
-                    "format": "none",
-                    "type": "number",
-                    "fieldType": "default",
-                    "minimum": 0
-                },
-                "proofOfException": {
-                    "bioAttributes": [],
-                    "fieldCategory": "evidence",
-                    "format": "none",
-                    "fieldType": "default",
-                    "$ref": "#\/definitions\/documentType"
-                },
-                "phone": {
-                    "bioAttributes": [],
-                    "validators": [
-                        {
-                            "validator": "^[+]*([0-9]{1})([0-9]{9})$",
-                            "arguments": [],
-                            "type": "regex"
-                        }
-                    ],
-                    "fieldCategory": "pvt",
-                    "format": "none",
-                    "type": "string",
-                    "fieldType": "default"
-                },
-                "introducerName": {
-                    "bioAttributes": [],
-                    "fieldCategory": "evidence",
-                    "format": "none",
-                    "fieldType": "default",
-                    "$ref": "#\/definitions\/simpleType"
-                },
-                "proofOfRelationship": {
-                    "bioAttributes": [],
-                    "fieldCategory": "pvt",
-                    "format": "none",
-                    "fieldType": "default",
-                    "$ref": "#\/definitions\/documentType"
-                },
-                "UIN": {
-                    "bioAttributes": [],
-                    "fieldCategory": "none",
-                    "format": "none",
-                    "type": "string",
-                    "fieldType": "default"
-                },
-                "preferredLang": {
-                    "bioAttributes": [],
-                    "fieldCategory": "pvt",
-                    "format": "none",
-                    "type": "string",
-                    "fieldType": "dynamic"
-                },
-                "region": {
-                    "bioAttributes": [],
-                    "validators": [
-                        {
-                            "validator": "^(?=.{0,50}$).*",
-                            "arguments": [],
-                            "type": "regex"
-                        }
-                    ],
-                    "fieldCategory": "pvt",
-                    "format": "none",
-                    "fieldType": "default",
-                    "$ref": "#\/definitions\/simpleType"
-                }
-            }
-        }
-    }
-}</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1020,12 +542,6 @@
       <sz val="11"/>
       <name val="Cambria"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1063,7 +579,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1079,9 +595,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1101,9 +614,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1141,7 +654,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1247,7 +760,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1389,7 +902,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1399,27 +912,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" style="1"/>
-    <col min="2" max="2" width="8.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.453125" style="1"/>
+    <col min="2" max="2" width="8.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.453125" style="1" customWidth="1"/>
     <col min="5" max="5" width="31" style="1" customWidth="1"/>
-    <col min="6" max="6" width="53.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="53.7265625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7265625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.453125" style="2" customWidth="1"/>
     <col min="9" max="9" width="10" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" style="2"/>
-    <col min="11" max="1023" width="8.42578125" style="1"/>
-    <col min="1024" max="1024" width="11.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.453125" style="2"/>
+    <col min="11" max="1023" width="8.453125" style="1"/>
+    <col min="1024" max="1024" width="11.54296875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1451,24 +962,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="274.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="C2" s="1">
         <v>0.1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>20</v>
+        <v>12</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>13</v>
@@ -1483,37 +994,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1001</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>16</v>
-      </c>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="1"/>
+      <c r="F3" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
[mosip-39781] changing idschema and UIspec for CRVS
Signed-off-by: khuddus shariff <khuddusshariff0022@gmail.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/identity_schema.xlsx
+++ b/mosip_master/xlsx/identity_schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB961A68-CEAC-4FB4-9EB6-1323E0FE1DB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5199A633-3BFB-49C1-809B-305816A3C1FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,7 +90,7 @@
     <t>CRVS sample identity</t>
   </si>
   <si>
-    <t>{"$schema":"http://json-schema.org/draft-07/schema#","description":"MOSIP Sample identity","additionalProperties":false,"title":"MOSIP identity","type":"object","definitions":{"simpleType":{"uniqueItems":true,"additionalItems":false,"type":"array","items":{"additionalProperties":false,"type":"object","required":["language","value"],"properties":{"language":{"type":"string"},"value":{"type":"string"}}}},"documentType":{"additionalProperties":false,"type":"object","properties":{"format":{"type":"string"},"type":{"type":"string"},"value":{"type":"string"},"refNumber":{"type":["string","null"]}}},"biometricsType":{"additionalProperties":false,"type":"object","properties":{"format":{"type":"string"},"version":{"type":"number","minimum":0},"value":{"type":"string"}}}},"properties":{"identity":{"additionalProperties":false,"type":"object","required":["IDSchemaVersion","fullName","dateOfBirth","gender","addressLine1","addressLine2","addressLine3","region","province","city","zone","postalCode","phone","email","proofOfIdentity","individualBiometrics"],"properties":{"proofOfAddress":{"bioAttributes":[],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#/definitions/documentType"},"gender":{"bioAttributes":[],"fieldCategory":"pvt","format":"","fieldType":"default","$ref":"#/definitions/simpleType"},"city":{"bioAttributes":[],"validators":[{"validator":"^(?=.{0,50}$).*","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#/definitions/simpleType"},"postalCode":{"bioAttributes":[],"validators":[{"validator":"^[(?i)A-Z0-9]{5}$|^NA$","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","type":"string","fieldType":"default"},"proofOfException-1":{"bioAttributes":[],"fieldCategory":"evidence","format":"none","fieldType":"default","$ref":"#/definitions/documentType"},"referenceIdentityNumber":{"bioAttributes":[],"validators":[{"validator":"^([0-9]{10,30})$","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"kyc","type":"string","fieldType":"default"},"individualBiometrics":{"bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#/definitions/biometricsType"},"province":{"bioAttributes":[],"validators":[{"validator":"^(?=.{0,50}$).*","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#/definitions/simpleType"},"zone":{"bioAttributes":[],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#/definitions/simpleType"},"proofOfDateOfBirth":{"bioAttributes":[],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#/definitions/documentType"},"addressLine1":{"bioAttributes":[],"validators":[{"validator":"^(?=.{0,50}$).*","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#/definitions/simpleType"},"addressLine2":{"bioAttributes":[],"validators":[{"validator":"^(?=.{3,50}$).*","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#/definitions/simpleType"},"residenceStatus":{"bioAttributes":[],"fieldCategory":"kyc","format":"none","fieldType":"default","$ref":"#/definitions/simpleType"},"addressLine3":{"bioAttributes":[],"validators":[{"validator":"^(?=.{3,50}$).*","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#/definitions/simpleType"},"email":{"bioAttributes":[],"validators":[{"validator":"^[A-Za-z0-9_\\-]+(\\.[A-Za-z0-9_]+)*@[A-Za-z0-9_-]+(\\.[A-Za-z0-9_]+)*(\\.[a-zA-Z]{2,})$","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","type":"string","fieldType":"default"},"introducerRID":{"bioAttributes":[],"fieldCategory":"evidence","format":"none","type":"string","fieldType":"default"},"introducerBiometrics":{"bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#/definitions/biometricsType"},"fullName":{"bioAttributes":[],"validators":[{"validator":"^(?=.{3,50}$).*","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#/definitions/simpleType"},"dateOfBirth":{"bioAttributes":[],"validators":[{"validator":"^(1869|18[7-9][0-9]|19[0-9][0-9]|20[0-9][0-9])/([0][1-9]|1[0-2])/([0][1-9]|[1-2][0-9]|3[01])$","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","type":"string","fieldType":"default"},"individualAuthBiometrics":{"bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#/definitions/biometricsType"},"introducerUIN":{"bioAttributes":[],"fieldCategory":"evidence","format":"none","type":"string","fieldType":"default"},"proofOfIdentity":{"bioAttributes":[],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#/definitions/documentType"},"IDSchemaVersion":{"bioAttributes":[],"fieldCategory":"none","format":"none","type":"number","fieldType":"default","minimum":0},"proofOfException":{"bioAttributes":[],"fieldCategory":"evidence","format":"none","fieldType":"default","$ref":"#/definitions/documentType"},"phone":{"bioAttributes":[],"validators":[{"validator":"^[+]*([0-9]{1})([0-9]{9})$","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","type":"string","fieldType":"default"},"introducerName":{"bioAttributes":[],"fieldCategory":"evidence","format":"none","fieldType":"default","$ref":"#/definitions/simpleType"},"proofOfRelationship":{"bioAttributes":[],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#/definitions/documentType"},"UIN":{"bioAttributes":[],"fieldCategory":"none","format":"none","type":"string","fieldType":"default"},"region":{"bioAttributes":[],"validators":[{"validator":"^(?=.{0,50}$).*","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#/definitions/simpleType"},"introducerInfoToken":{"bioAttributes":[],"fieldCategory":"evidence","format":"none","type":"string","fieldType":"default"},"deceasedInformer ":{"bioAttributes":[],"fieldCategory":"evidence","format":"none","type":"string","fieldType":"default"},"deceasedDeclarationDate ":{"bioAttributes":[],"validators":[{"validator":"^(1869|18[7-9][0-9]|19[0-9][0-9]|20[0-9][0-9])/([0][1-9]|1[0-2])/([0][1-9]|[1-2][0-9]|3[01])$","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","type":"string","fieldType":"default"},"declaredAsDeceased ":{"bioAttributes":[],"validators":[{"validator":"^(y|n)$","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","type":"string","fieldType":"default"},"typeOfDeath ":{"bioAttributes":[],"fieldCategory":"pvt","format":"none","type":"string","fieldType":"default"}}}}}</t>
+    <t>{"$schema":"http:\/\/json-schema.org\/draft-07\/schema#","description":"MOSIP Sample identity","additionalProperties":false,"title":"MOSIP identity","type":"object","definitions":{"simpleType":{"uniqueItems":true,"additionalItems":false,"type":"array","items":{"additionalProperties":false,"type":"object","required":["language","value"],"properties":{"language":{"type":"string"},"value":{"type":"string"}}}},"documentType":{"additionalProperties":false,"type":"object","properties":{"format":{"type":"string"},"type":{"type":"string"},"value":{"type":"string"},"refNumber":{"type":["string","null"]}}},"biometricsType":{"additionalProperties":false,"type":"object","properties":{"format":{"type":"string"},"version":{"type":"number","minimum":0},"value":{"type":"string"}}}},"properties":{"identity":{"additionalProperties":false,"type":"object","required":["IDSchemaVersion","fullName","dateOfBirth","gender","addressLine1","addressLine2","addressLine3","region","province","city","zone","postalCode","phone","email","proofOfIdentity","individualBiometrics"],"properties":{"proofOfAddress":{"bioAttributes":[],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/documentType"},"gender":{"bioAttributes":[],"fieldCategory":"pvt","format":"","fieldType":"default","$ref":"#\/definitions\/simpleType"},"city":{"bioAttributes":[],"validators":[{"validator":"^(?=.{0,50}$).*","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/simpleType"},"postalCode":{"bioAttributes":[],"validators":[{"validator":"^[(?i)A-Z0-9]{5}$|^NA$","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","type":"string","fieldType":"default"},"proofOfException-1":{"bioAttributes":[],"fieldCategory":"evidence","format":"none","fieldType":"default","$ref":"#\/definitions\/documentType"},"referenceIdentityNumber":{"bioAttributes":[],"validators":[{"validator":"^([0-9]{10,30})$","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"kyc","type":"string","fieldType":"default"},"individualBiometrics":{"bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/biometricsType"},"province":{"bioAttributes":[],"validators":[{"validator":"^(?=.{0,50}$).*","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/simpleType"},"zone":{"bioAttributes":[],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/simpleType"},"proofOfDateOfBirth":{"bioAttributes":[],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/documentType"},"addressLine1":{"bioAttributes":[],"validators":[{"validator":"^(?=.{0,50}$).*","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/simpleType"},"addressLine2":{"bioAttributes":[],"validators":[{"validator":"^(?=.{3,50}$).*","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/simpleType"},"residenceStatus":{"bioAttributes":[],"fieldCategory":"kyc","format":"none","fieldType":"default","$ref":"#\/definitions\/simpleType"},"addressLine3":{"bioAttributes":[],"validators":[{"validator":"^(?=.{3,50}$).*","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/simpleType"},"email":{"bioAttributes":[],"validators":[{"validator":"^[A-Za-z0-9_\\-]+(\\.[A-Za-z0-9_]+)*@[A-Za-z0-9_-]+(\\.[A-Za-z0-9_]+)*(\\.[a-zA-Z]{2,})$","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","type":"string","fieldType":"default"},"introducerRID":{"bioAttributes":[],"fieldCategory":"evidence","format":"none","type":"string","fieldType":"default"},"introducerBiometrics":{"bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/biometricsType"},"fullName":{"bioAttributes":[],"validators":[{"validator":"^(?=.{3,50}$).*","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/simpleType"},"dateOfBirth":{"bioAttributes":[],"validators":[{"validator":"^(1869|18[7-9][0-9]|19[0-9][0-9]|20[0-9][0-9])\/([0][1-9]|1[0-2])\/([0][1-9]|[1-2][0-9]|3[01])$","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","type":"string","fieldType":"default"},"individualAuthBiometrics":{"bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/biometricsType"},"introducerUIN":{"bioAttributes":[],"fieldCategory":"evidence","format":"none","type":"string","fieldType":"default"},"proofOfIdentity":{"bioAttributes":[],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/documentType"},"IDSchemaVersion":{"bioAttributes":[],"fieldCategory":"none","format":"none","type":"number","fieldType":"default","minimum":0},"proofOfException":{"bioAttributes":[],"fieldCategory":"evidence","format":"none","fieldType":"default","$ref":"#\/definitions\/documentType"},"phone":{"bioAttributes":[],"validators":[{"validator":"^[+]*([0-9]{1})([0-9]{9})$","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","type":"string","fieldType":"default"},"introducerName":{"bioAttributes":[],"fieldCategory":"evidence","format":"none","fieldType":"default","$ref":"#\/definitions\/simpleType"},"proofOfRelationship":{"bioAttributes":[],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/documentType"},"UIN":{"bioAttributes":[],"fieldCategory":"none","format":"none","type":"string","fieldType":"default"},"region":{"bioAttributes":[],"validators":[{"validator":"^(?=.{0,50}$).*","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","fieldType":"default","$ref":"#\/definitions\/simpleType"},"introducerInfoToken":{"bioAttributes":[],"fieldCategory":"evidence","format":"none","type":"string","fieldType":"default"},"deceasedInformer ":{"bioAttributes":[],"fieldCategory":"evidence","format":"none","type":"string","fieldType":"default"},"deceasedDeclarationDate ":{"bioAttributes":[],"validators":[{"validator":"^(1869|18[7-9][0-9]|19[0-9][0-9]|20[0-9][0-9])/([0][1-9]|1[0-2])/([0][1-9]|[1-2][0-9]|3[01])$","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","type":"string","fieldType":"default"},"declaredAsDeceased ":{"bioAttributes":[],"validators":[{"validator":"^(Y|N)$","arguments":[],"type":"regex"}],"fieldCategory":"pvt","format":"none","type":"string","fieldType":"default"},"typeOfDeath ":{"bioAttributes":[],"fieldCategory":"pvt","format":"none","type":"string","fieldType":"default"}}}}}</t>
   </si>
 </sst>
 </file>
@@ -483,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated identity_schema with CRVS attributes
Signed-off-by: Chetan Kumar Hirematha <chetankumar.h.239@gmail.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/identity_schema.xlsx
+++ b/mosip_master/xlsx/identity_schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gokulraj\Documents\GitHub\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\Mosip\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7CA555-3A71-455F-823C-825C0E4FF772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12221C01-E901-4B51-8184-E68A983A3D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -76,453 +76,6 @@
   </si>
   <si>
     <t>TRUE</t>
-  </si>
-  <si>
-    <t>{
-	"$schema": "http:\/\/json-schema.org\/draft-07\/schema#",
-	"description": "MOSIP Sample identity",
-	"additionalProperties": false,
-	"title": "MOSIP identity",
-	"type": "object",
-	"definitions": {
-		"simpleType": {
-			"uniqueItems": true,
-			"additionalItems": false,
-			"type": "array",
-			"items": {
-				"additionalProperties": false,
-				"type": "object",
-				"required": [
-					"language",
-					"value"
-				],
-				"properties": {
-					"language": {
-						"type": "string"
-					},
-					"value": {
-						"type": "string"
-					}
-				}
-			}
-		},
-		"documentType": {
-			"additionalProperties": false,
-			"type": "object",
-			"properties": {
-				"format": {
-					"type": "string"
-				},
-				"type": {
-					"type": "string"
-				},
-				"value": {
-					"type": "string"
-				},
-				"refNumber": {
-					"type": [
-						"string",
-						"null"
-					]
-				}
-			}
-		},
-		"biometricsType": {
-			"additionalProperties": false,
-			"type": "object",
-			"properties": {
-				"format": {
-					"type": "string"
-				},
-				"version": {
-					"type": "number",
-					"minimum": 0
-				},
-				"value": {
-					"type": "string"
-				}
-			}
-		}
-	},
-	"properties": {
-		"identity": {
-			"additionalProperties": false,
-			"type": "object",
-			"required": [
-				"IDSchemaVersion",
-				"fullName",
-				"dateOfBirth",
-				"gender",
-				"addressLine1",
-				"addressLine2",
-				"addressLine3",
-				"region",
-				"province",
-				"city",
-				"zone",
-				"postalCode",
-				"phone",
-				"email",
-				"proofOfIdentity",
-				"individualBiometrics"
-			],
-			"properties": {
-				"proofOfAddress": {
-					"bioAttributes": [
-					],
-					"fieldCategory": "pvt",
-					"format": "none",
-					"fieldType": "default",
-					"$ref": "#\/definitions\/documentType"
-				},
-				"gender": {
-					"bioAttributes": [
-					],
-					"fieldCategory": "pvt",
-					"format": "",
-					"fieldType": "default",
-					"$ref": "#\/definitions\/simpleType"
-				},
-				"city": {
-					"bioAttributes": [
-					],
-					"validators": [{
-						"validator": "^(?=.{0,50}$).*",
-						"arguments": [
-						],
-						"type": "regex"
-					}],
-					"fieldCategory": "pvt",
-					"format": "none",
-					"fieldType": "default",
-					"$ref": "#\/definitions\/simpleType"
-				},
-				"postalCode": {
-					"bioAttributes": [
-					],
-					"validators": [{
-						"validator": "^[(?i)A-Z0-9]{5}$|^NA$",
-						"arguments": [
-						],
-						"type": "regex"
-					}],
-					"fieldCategory": "pvt",
-					"format": "none",
-					"type": "string",
-					"fieldType": "default"
-				},
-				"proofOfException-1": {
-					"bioAttributes": [
-					],
-					"fieldCategory": "evidence",
-					"format": "none",
-					"fieldType": "default",
-					"$ref": "#\/definitions\/documentType"
-				},
-				"referenceIdentityNumber": {
-					"bioAttributes": [
-					],
-					"validators": [{
-						"validator": "^([0-9]{10,30})$",
-						"arguments": [
-						],
-						"type": "regex"
-					}],
-					"fieldCategory": "pvt",
-					"format": "kyc",
-					"type": "string",
-					"fieldType": "default"
-				},
-				"individualBiometrics": {
-					"bioAttributes": [
-						"leftEye",
-						"rightEye",
-						"rightIndex",
-						"rightLittle",
-						"rightRing",
-						"rightMiddle",
-						"leftIndex",
-						"leftLittle",
-						"leftRing",
-						"leftMiddle",
-						"leftThumb",
-						"rightThumb",
-						"face"
-					],
-					"fieldCategory": "pvt",
-					"format": "none",
-					"fieldType": "default",
-					"$ref": "#\/definitions\/biometricsType"
-				},
-				"province": {
-					"bioAttributes": [
-					],
-					"validators": [{
-						"validator": "^(?=.{0,50}$).*",
-						"arguments": [
-						],
-						"type": "regex"
-					}],
-					"fieldCategory": "pvt",
-					"format": "none",
-					"fieldType": "default",
-					"$ref": "#\/definitions\/simpleType"
-				},
-				"zone": {
-					"bioAttributes": [
-					],
-					"fieldCategory": "pvt",
-					"format": "none",
-					"fieldType": "default",
-					"$ref": "#\/definitions\/simpleType"
-				},
-				"proofOfDateOfBirth": {
-					"bioAttributes": [
-					],
-					"fieldCategory": "pvt",
-					"format": "none",
-					"fieldType": "default",
-					"$ref": "#\/definitions\/documentType"
-				},
-				"addressLine1": {
-					"bioAttributes": [
-					],
-					"validators": [{
-						"validator": "^(?=.{0,50}$).*",
-						"arguments": [
-						],
-						"type": "regex"
-					}],
-					"fieldCategory": "pvt",
-					"format": "none",
-					"fieldType": "default",
-					"$ref": "#\/definitions\/simpleType"
-				},
-				"addressLine2": {
-					"bioAttributes": [
-					],
-					"validators": [{
-						"validator": "^(?=.{3,50}$).*",
-						"arguments": [
-						],
-						"type": "regex"
-					}],
-					"fieldCategory": "pvt",
-					"format": "none",
-					"fieldType": "default",
-					"$ref": "#\/definitions\/simpleType"
-				},
-				"residenceStatus": {
-					"bioAttributes": [
-					],
-					"fieldCategory": "kyc",
-					"format": "none",
-					"fieldType": "default",
-					"$ref": "#\/definitions\/simpleType"
-				},
-				"addressLine3": {
-					"bioAttributes": [
-					],
-					"validators": [{
-						"validator": "^(?=.{3,50}$).*",
-						"arguments": [
-						],
-						"type": "regex"
-					}],
-					"fieldCategory": "pvt",
-					"format": "none",
-					"fieldType": "default",
-					"$ref": "#\/definitions\/simpleType"
-				},
-				"email": {
-					"bioAttributes": [
-					],
-					"validators": [{
-						"validator": "^[A-Za-z0-9_\\-]+(\\.[A-Za-z0-9_]+)*@[A-Za-z0-9_-]+(\\.[A-Za-z0-9_]+)*(\\.[a-zA-Z]{2,})$",
-						"arguments": [
-						],
-						"type": "regex"
-					}],
-					"fieldCategory": "pvt",
-					"format": "none",
-					"type": "string",
-					"fieldType": "default"
-				},
-				"introducerRID": {
-					"bioAttributes": [
-					],
-					"fieldCategory": "evidence",
-					"format": "none",
-					"type": "string",
-					"fieldType": "default"
-				},
-				"introducerBiometrics": {
-					"bioAttributes": [
-						"leftEye",
-						"rightEye",
-						"rightIndex",
-						"rightLittle",
-						"rightRing",
-						"rightMiddle",
-						"leftIndex",
-						"leftLittle",
-						"leftRing",
-						"leftMiddle",
-						"leftThumb",
-						"rightThumb",
-						"face"
-					],
-					"fieldCategory": "pvt",
-					"format": "none",
-					"fieldType": "default",
-					"$ref": "#\/definitions\/biometricsType"
-				},
-				"fullName": {
-					"bioAttributes": [
-					],
-					"validators": [{
-						"validator": "^(?=.{3,50}$).*",
-						"arguments": [
-						],
-						"type": "regex"
-					}],
-					"fieldCategory": "pvt",
-					"format": "none",
-					"fieldType": "default",
-					"$ref": "#\/definitions\/simpleType"
-				},
-				"dateOfBirth": {
-					"bioAttributes": [
-					],
-					"validators": [{
-						"validator": "^(1869|18[7-9][0-9]|19[0-9][0-9]|20[0-9][0-9])\/([0][1-9]|1[0-2])\/([0][1-9]|[1-2][0-9]|3[01])$",
-						"arguments": [
-						],
-						"type": "regex"
-					}],
-					"fieldCategory": "pvt",
-					"format": "none",
-					"type": "string",
-					"fieldType": "default"
-				},
-				"individualAuthBiometrics": {
-					"bioAttributes": [
-						"leftEye",
-						"rightEye",
-						"rightIndex",
-						"rightLittle",
-						"rightRing",
-						"rightMiddle",
-						"leftIndex",
-						"leftLittle",
-						"leftRing",
-						"leftMiddle",
-						"leftThumb",
-						"rightThumb",
-						"face"
-					],
-					"fieldCategory": "pvt",
-					"format": "none",
-					"fieldType": "default",
-					"$ref": "#\/definitions\/biometricsType"
-				},
-				"introducerUIN": {
-					"bioAttributes": [
-					],
-					"fieldCategory": "evidence",
-					"format": "none",
-					"type": "string",
-					"fieldType": "default"
-				},
-				"proofOfIdentity": {
-					"bioAttributes": [
-					],
-					"fieldCategory": "pvt",
-					"format": "none",
-					"fieldType": "default",
-					"$ref": "#\/definitions\/documentType"
-				},
-				"IDSchemaVersion": {
-					"bioAttributes": [
-					],
-					"fieldCategory": "none",
-					"format": "none",
-					"type": "number",
-					"fieldType": "default",
-					"minimum": 0
-				},
-				"proofOfException": {
-					"bioAttributes": [
-					],
-					"fieldCategory": "evidence",
-					"format": "none",
-					"fieldType": "default",
-					"$ref": "#\/definitions\/documentType"
-				},
-				"phone": {
-					"bioAttributes": [
-					],
-					"validators": [{
-						"validator": "^[+]*([0-9]{1})([0-9]{9})$",
-						"arguments": [
-						],
-						"type": "regex"
-					}],
-					"fieldCategory": "pvt",
-					"format": "none",
-					"type": "string",
-					"fieldType": "default"
-				},
-				"introducerName": {
-					"bioAttributes": [
-					],
-					"fieldCategory": "evidence",
-					"format": "none",
-					"fieldType": "default",
-					"$ref": "#\/definitions\/simpleType"
-				},
-				"proofOfRelationship": {
-					"bioAttributes": [
-					],
-					"fieldCategory": "pvt",
-					"format": "none",
-					"fieldType": "default",
-					"$ref": "#\/definitions\/documentType"
-				},
-				"UIN": {
-					"bioAttributes": [
-					],
-					"fieldCategory": "none",
-					"format": "none",
-					"type": "string",
-					"fieldType": "default"
-				},
-				"preferredLang": {
-					"bioAttributes": [
-					],
-					"fieldCategory": "pvt",
-					"format": "none",
-					"type": "string",
-					"fieldType": "dynamic"
-				},
-				"region": {
-					"bioAttributes": [
-					],
-					"validators": [{
-						"validator": "^(?=.{0,50}$).*",
-						"arguments": [
-						],
-						"type": "regex"
-					}],
-					"fieldCategory": "pvt",
-					"format": "none",
-					"fieldType": "default",
-					"$ref": "#\/definitions\/simpleType"
-				}
-			}
-		}
-	}
-}</t>
   </si>
   <si>
     <t>Mosip Sample identity for handle</t>
@@ -996,6 +549,533 @@
                     "format": "none",
                     "fieldType": "default",
                     "$ref": "#\/definitions\/simpleType"
+                }
+            }
+        }
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "$schema": "http://json-schema.org/draft-07/schema#",
+    "description": "MOSIP Sample identity",
+    "additionalProperties": false,
+    "title": "MOSIP identity",
+    "type": "object",
+    "definitions": {
+        "simpleType": {
+            "uniqueItems": true,
+            "additionalItems": false,
+            "type": "array",
+            "items": {
+                "additionalProperties": false,
+                "type": "object",
+                "required": [
+                    "language",
+                    "value"
+                ],
+                "properties": {
+                    "language": {
+                        "type": "string"
+                    },
+                    "value": {
+                        "type": "string"
+                    }
+                }
+            }
+        },
+        "documentType": {
+            "additionalProperties": false,
+            "type": "object",
+            "properties": {
+                "format": {
+                    "type": "string"
+                },
+                "type": {
+                    "type": "string"
+                },
+                "value": {
+                    "type": "string"
+                },
+                "refNumber": {
+                    "type": [
+                        "string",
+                        "null"
+                    ]
+                }
+            }
+        },
+        "biometricsType": {
+            "additionalProperties": false,
+            "type": "object",
+            "properties": {
+                "format": {
+                    "type": "string"
+                },
+                "version": {
+                    "type": "number",
+                    "minimum": 0
+                },
+                "value": {
+                    "type": "string"
+                }
+            }
+        }
+    },
+    "properties": {
+        "identity": {
+            "additionalProperties": false,
+            "type": "object",
+            "required": [
+                "IDSchemaVersion",
+                "fullName",
+                "dateOfBirth",
+                "gender",
+                "addressLine1",
+                "addressLine2",
+                "addressLine3",
+                "region",
+                "province",
+                "city",
+                "zone",
+                "postalCode",
+                "phone",
+                "email",
+                "proofOfIdentity",
+                "individualBiometrics"
+            ],
+            "properties": {
+                "proofOfAddress": {
+                    "bioAttributes": [
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#/definitions/documentType"
+                },
+                "gender": {
+                    "bioAttributes": [
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "",
+                    "fieldType": "default",
+                    "$ref": "#/definitions/simpleType"
+                },
+                "city": {
+                    "bioAttributes": [
+                    ],
+                    "validators": [
+                        {
+                            "validator": "^(?=.{0,50}$).*",
+                            "arguments": [
+                            ],
+                            "type": "regex"
+                        }
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#/definitions/simpleType"
+                },
+                "postalCode": {
+                    "bioAttributes": [
+                    ],
+                    "validators": [
+                        {
+                            "validator": "^[(?i)A-Z0-9]{5}$|^NA$",
+                            "arguments": [
+                            ],
+                            "type": "regex"
+                        }
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "type": "string",
+                    "fieldType": "default"
+                },
+                "proofOfException-1": {
+                    "bioAttributes": [
+                    ],
+                    "fieldCategory": "evidence",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#/definitions/documentType"
+                },
+                "referenceIdentityNumber": {
+                    "bioAttributes": [
+                    ],
+                    "validators": [
+                        {
+                            "validator": "^([0-9]{10,30})$",
+                            "arguments": [
+                            ],
+                            "type": "regex"
+                        }
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "kyc",
+                    "type": "string",
+                    "fieldType": "default"
+                },
+                "individualBiometrics": {
+                    "bioAttributes": [
+                        "leftEye",
+                        "rightEye",
+                        "rightIndex",
+                        "rightLittle",
+                        "rightRing",
+                        "rightMiddle",
+                        "leftIndex",
+                        "leftLittle",
+                        "leftRing",
+                        "leftMiddle",
+                        "leftThumb",
+                        "rightThumb",
+                        "face"
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#/definitions/biometricsType"
+                },
+                "province": {
+                    "bioAttributes": [
+                    ],
+                    "validators": [
+                        {
+                            "validator": "^(?=.{0,50}$).*",
+                            "arguments": [
+                            ],
+                            "type": "regex"
+                        }
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#/definitions/simpleType"
+                },
+                "zone": {
+                    "bioAttributes": [
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#/definitions/simpleType"
+                },
+                "proofOfDateOfBirth": {
+                    "bioAttributes": [
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#/definitions/documentType"
+                },
+                "addressLine1": {
+                    "bioAttributes": [
+                    ],
+                    "validators": [
+                        {
+                            "validator": "^(?=.{0,50}$).*",
+                            "arguments": [
+                            ],
+                            "type": "regex"
+                        }
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#/definitions/simpleType"
+                },
+                "addressLine2": {
+                    "bioAttributes": [
+                    ],
+                    "validators": [
+                        {
+                            "validator": "^(?=.{3,50}$).*",
+                            "arguments": [
+                            ],
+                            "type": "regex"
+                        }
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#/definitions/simpleType"
+                },
+                "residenceStatus": {
+                    "bioAttributes": [
+                    ],
+                    "fieldCategory": "kyc",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#/definitions/simpleType"
+                },
+                "addressLine3": {
+                    "bioAttributes": [
+                    ],
+                    "validators": [
+                        {
+                            "validator": "^(?=.{3,50}$).*",
+                            "arguments": [
+                            ],
+                            "type": "regex"
+                        }
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#/definitions/simpleType"
+                },
+                "email": {
+                    "bioAttributes": [
+                    ],
+                    "validators": [
+                        {
+                            "validator": "^[A-Za-z0-9_\\-]+(\\.[A-Za-z0-9_]+)*@[A-Za-z0-9_-]+(\\.[A-Za-z0-9_]+)*(\\.[a-zA-Z]{2,})$",
+                            "arguments": [
+                            ],
+                            "type": "regex"
+                        }
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "type": "string",
+                    "fieldType": "default"
+                },
+                "introducerRID": {
+                    "bioAttributes": [
+                    ],
+                    "fieldCategory": "evidence",
+                    "format": "none",
+                    "type": "string",
+                    "fieldType": "default"
+                },
+                "introducerBiometrics": {
+                    "bioAttributes": [
+                        "leftEye",
+                        "rightEye",
+                        "rightIndex",
+                        "rightLittle",
+                        "rightRing",
+                        "rightMiddle",
+                        "leftIndex",
+                        "leftLittle",
+                        "leftRing",
+                        "leftMiddle",
+                        "leftThumb",
+                        "rightThumb",
+                        "face"
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#/definitions/biometricsType"
+                },
+                "fullName": {
+                    "bioAttributes": [
+                    ],
+                    "validators": [
+                        {
+                            "validator": "^(?=.{3,50}$).*",
+                            "arguments": [
+                            ],
+                            "type": "regex"
+                        }
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#/definitions/simpleType"
+                },
+                "dateOfBirth": {
+                    "bioAttributes": [
+                    ],
+                    "validators": [
+                        {
+                            "validator": "^(1869|18[7-9][0-9]|19[0-9][0-9]|20[0-9][0-9])/([0][1-9]|1[0-2])/([0][1-9]|[1-2][0-9]|3[01])$",
+                            "arguments": [
+                            ],
+                            "type": "regex"
+                        }
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "type": "string",
+                    "fieldType": "default"
+                },
+                "individualAuthBiometrics": {
+                    "bioAttributes": [
+                        "leftEye",
+                        "rightEye",
+                        "rightIndex",
+                        "rightLittle",
+                        "rightRing",
+                        "rightMiddle",
+                        "leftIndex",
+                        "leftLittle",
+                        "leftRing",
+                        "leftMiddle",
+                        "leftThumb",
+                        "rightThumb",
+                        "face"
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#/definitions/biometricsType"
+                },
+                "introducerUIN": {
+                    "bioAttributes": [
+                    ],
+                    "fieldCategory": "evidence",
+                    "format": "none",
+                    "type": "string",
+                    "fieldType": "default"
+                },
+                "proofOfIdentity": {
+                    "bioAttributes": [
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#/definitions/documentType"
+                },
+                "IDSchemaVersion": {
+                    "bioAttributes": [
+                    ],
+                    "fieldCategory": "none",
+                    "format": "none",
+                    "type": "number",
+                    "fieldType": "default",
+                    "minimum": 0
+                },
+                "proofOfException": {
+                    "bioAttributes": [
+                    ],
+                    "fieldCategory": "evidence",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#/definitions/documentType"
+                },
+                "phone": {
+                    "bioAttributes": [
+                    ],
+                    "validators": [
+                        {
+                            "validator": "^[+]*([0-9]{1})([0-9]{9})$",
+                            "arguments": [
+                            ],
+                            "type": "regex"
+                        }
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "type": "string",
+                    "fieldType": "default"
+                },
+                "introducerName": {
+                    "bioAttributes": [
+                    ],
+                    "fieldCategory": "evidence",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#/definitions/simpleType"
+                },
+                "proofOfRelationship": {
+                    "bioAttributes": [
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#/definitions/documentType"
+                },
+                "UIN": {
+                    "bioAttributes": [
+                    ],
+                    "fieldCategory": "none",
+                    "format": "none",
+                    "type": "string",
+                    "fieldType": "default"
+                },
+                "preferredLang": {
+                    "bioAttributes": [
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "type": "string",
+                    "fieldType": "dynamic"
+                },
+                "region": {
+                    "bioAttributes": [
+                    ],
+                    "validators": [
+                        {
+                            "validator": "^(?=.{0,50}$).*",
+                            "arguments": [
+                            ],
+                            "type": "regex"
+                        }
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#/definitions/simpleType"
+                },
+                "introducerInfoToken": {
+                    "bioAttributes": [
+                    ],
+                    "fieldCategory": "evidence",
+                    "format": "none",
+                    "type": "string",
+                    "fieldType": "default"
+                },
+                "deceasedInformer": {
+                    "bioAttributes": [
+                    ],
+                    "fieldCategory": "evidence",
+                    "format": "none",
+                    "type": "string",
+                    "fieldType": "default"
+                },
+                "deceasedDeclarationDate": {
+                    "bioAttributes": [
+                    ],
+                    "validators": [
+                        {
+                            "validator": "^(1869|18[7-9][0-9]|19[0-9][0-9]|20[0-9][0-9])/([0][1-9]|1[0-2])/([0][1-9]|[1-2][0-9]|3[01])$",
+                            "arguments": [
+                            ],
+                            "type": "regex"
+                        }
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "type": "string",
+                    "fieldType": "default"
+                },
+                "declaredAsDeceased": {
+                    "bioAttributes": [
+                    ],
+                    "validators": [
+                        {
+                            "validator": "^(Y|N)$",
+                            "arguments": [
+                            ],
+                            "type": "regex"
+                        }
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "type": "string",
+                    "fieldType": "default"
+                },
+                "typeOfDeath": {
+                    "bioAttributes": [
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "type": "string",
+                    "fieldType": "default"
                 }
             }
         }
@@ -1399,27 +1479,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" style="1"/>
-    <col min="2" max="2" width="8.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.453125" style="1"/>
+    <col min="2" max="2" width="8.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.453125" style="1" customWidth="1"/>
     <col min="5" max="5" width="31" style="1" customWidth="1"/>
-    <col min="6" max="6" width="53.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="53.7265625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7265625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.453125" style="2" customWidth="1"/>
     <col min="9" max="9" width="10" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" style="2"/>
-    <col min="11" max="1023" width="8.42578125" style="1"/>
-    <col min="1024" max="1024" width="11.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.453125" style="2"/>
+    <col min="11" max="1023" width="8.453125" style="1"/>
+    <col min="1024" max="1024" width="11.54296875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1451,7 +1531,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="274.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="274.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1462,13 +1542,13 @@
         <v>0.1</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>13</v>
@@ -1483,7 +1563,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1491,7 +1571,7 @@
         <v>1001</v>
       </c>
       <c r="C3" s="1">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -1500,7 +1580,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Reverted back version with 0.2
Signed-off-by: Chetan Kumar Hirematha <chetankumar.h.239@gmail.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/identity_schema.xlsx
+++ b/mosip_master/xlsx/identity_schema.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\Mosip\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12221C01-E901-4B51-8184-E68A983A3D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6853C445-E25F-430A-8E58-44DFBBB35A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -1480,7 +1480,7 @@
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1571,7 +1571,7 @@
         <v>1001</v>
       </c>
       <c r="C3" s="1">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
MOSIP-35360 - packetCreatedOn added in identity_schema
Signed-off-by: Nidhi0201 <nidhi.k@cyberpwn.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/identity_schema.xlsx
+++ b/mosip_master/xlsx/identity_schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA486A0-4016-4BD7-9AA3-56B98C58C442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69913C26-673E-490F-8A2D-E108E0958E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -518,7 +518,15 @@
 					"format": "none",
 					"fieldType": "default",
 					"$ref": "#\/definitions\/simpleType"
-				}
+				},
+				"packetCreatedOn": {
+                    "bioAttributes": [
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "type": "string",
+                    "fieldType": "default"
+                }
 			}
 		}
 	}
@@ -614,9 +622,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -654,7 +662,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -760,7 +768,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -902,7 +910,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -912,7 +920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[MOSIP-43633] Added packetCreatedOn to identity schema for biometric issue fix
Signed-off-by: Ashok Kumar Sharma <ashok@mosip.io>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/identity_schema.xlsx
+++ b/mosip_master/xlsx/identity_schema.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\Mosip\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MOSIP_Project_Code\Repositories\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E632B33-EFBA-45CC-B1A2-807AF397E164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802CDE44-E0A3-4C0C-A167-43C6FAB26EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -568,6 +568,14 @@
                     "fieldType": "default"
                 },
                 "typeOfDeath": {
+                    "bioAttributes": [
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "type": "string",
+                    "fieldType": "default"
+                },
+				"packetCreatedOn": {
                     "bioAttributes": [
                     ],
                     "fieldCategory": "pvt",
@@ -670,9 +678,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -710,7 +718,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -816,7 +824,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -958,7 +966,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>

</xml_diff>

<commit_message>
[MOSIP-43633] Added packetCreatedOn to identity schema for biometric issue fix in develop branch
Signed-off-by: Ashok Kumar Sharma <ashok@mosip.io>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/identity_schema.xlsx
+++ b/mosip_master/xlsx/identity_schema.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\Mosip\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MOSIP_Project_Code\Repositories\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5F577B-0FC1-4AB5-BC48-3A9302F4BF07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581047B6-D335-4143-9889-A8A6BC002139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1046,6 +1046,14 @@
                     "fieldType": "default"
                 },
                 "typeOfDeath": {
+                    "bioAttributes": [
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "type": "string",
+                    "fieldType": "default"
+                },
+				"packetCreatedOn": {
                     "bioAttributes": [
                     ],
                     "fieldCategory": "pvt",
@@ -1157,9 +1165,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1197,7 +1205,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1303,7 +1311,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1445,7 +1453,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1456,7 +1464,7 @@
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Revert "[MOSIP-43633] Added packetCreatedOn to identity schema for biometric issue fix"
Signed-off-by: ashok-ksharma <ashok@mosip.io>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/identity_schema.xlsx
+++ b/mosip_master/xlsx/identity_schema.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MOSIP_Project_Code\Repositories\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\Mosip\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802CDE44-E0A3-4C0C-A167-43C6FAB26EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E632B33-EFBA-45CC-B1A2-807AF397E164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -568,14 +568,6 @@
                     "fieldType": "default"
                 },
                 "typeOfDeath": {
-                    "bioAttributes": [
-                    ],
-                    "fieldCategory": "pvt",
-                    "format": "none",
-                    "type": "string",
-                    "fieldType": "default"
-                },
-				"packetCreatedOn": {
                     "bioAttributes": [
                     ],
                     "fieldCategory": "pvt",
@@ -678,9 +670,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -718,7 +710,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -824,7 +816,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -966,7 +958,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>

</xml_diff>